<commit_message>
feito alteração no valor da parcela x
</commit_message>
<xml_diff>
--- a/finan.xlsx
+++ b/finan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/paulo_cainelles_prestserv_petrobras_com_br/Documents/Documentos/GitHub/planejamento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="8_{EC1AC212-DB19-4848-888C-E47EB9D93AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4BF563F-8AA7-42C9-A55B-E1EB485B4574}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{EC1AC212-DB19-4848-888C-E47EB9D93AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A8B20D3-F00E-485C-AA24-9A705ABD3BC7}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{4FBCED0E-6C2B-4F10-A7DA-909F50FE71FD}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="16410" windowHeight="15345" xr2:uid="{4FBCED0E-6C2B-4F10-A7DA-909F50FE71FD}"/>
   </bookViews>
   <sheets>
     <sheet name="SAIDAS" sheetId="1" r:id="rId1"/>
@@ -936,7 +936,7 @@
   <dimension ref="A1:P5225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H3" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="33">
-        <v>350</v>
+        <v>320</v>
       </c>
       <c r="F2" s="32"/>
     </row>

</xml_diff>